<commit_message>
fano factor 3d plotting plotly
</commit_message>
<xml_diff>
--- a/code/test/dataframes/Pandas000.xlsx
+++ b/code/test/dataframes/Pandas000.xlsx
@@ -404,628 +404,628 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c s="1" t="s" r="B1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c s="1" t="s" r="C1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c s="1" t="s" r="D1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c s="1" t="s" r="E1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c s="1" t="n" r="A2">
-        <v>0.03457546063131148</v>
+        <v>0.14851510907452498</v>
       </c>
       <c t="n" r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c t="n" r="D2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c s="1" t="n" r="A3">
-        <v>0.03784856577422081</v>
+        <v>0.14912278089866118</v>
       </c>
       <c t="n" r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c t="n" r="C3">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c t="n" r="D3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E3">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c s="1" t="n" r="A4">
-        <v>0.04068361270046923</v>
+        <v>0.19037965090090636</v>
       </c>
       <c t="n" r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C4">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c t="n" r="D4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E4">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c s="1" t="n" r="A5">
-        <v>0.04155309047786392</v>
+        <v>0.1143382949222053</v>
       </c>
       <c t="n" r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c t="n" r="D5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c s="1" t="n" r="A6">
-        <v>0.046328936639688435</v>
+        <v>0.03784856577422081</v>
       </c>
       <c t="n" r="B6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c t="n" r="C6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="D6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c t="n" r="E6">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c s="1" t="n" r="A7">
-        <v>0.050765735646263285</v>
+        <v>0.1659653838406194</v>
       </c>
       <c t="n" r="B7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C7">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c t="n" r="D7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E7">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c s="1" t="n" r="A8">
-        <v>0.0592547579755059</v>
+        <v>0.046328936639688435</v>
       </c>
       <c t="n" r="B8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C8">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c t="n" r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c t="n" r="E8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c s="1" t="n" r="A9">
-        <v>0.060400417357177216</v>
+        <v>0.04155309047786392</v>
       </c>
       <c t="n" r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c t="n" r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="D9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c t="n" r="E9">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c s="1" t="n" r="A10">
-        <v>0.06410720499822353</v>
+        <v>0.08681094419864815</v>
       </c>
       <c t="n" r="B10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="D10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c t="n" r="E10">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c s="1" t="n" r="A11">
-        <v>0.08489057724821769</v>
+        <v>0.12971370597969578</v>
       </c>
       <c t="n" r="B11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C11">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E11">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c s="1" t="n" r="A12">
-        <v>0.08597586519514165</v>
+        <v>0.04068361270046923</v>
       </c>
       <c t="n" r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c t="n" r="C12">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="E12">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c s="1" t="n" r="A13">
-        <v>0.08681094419864815</v>
+        <v>0.24919639115256959</v>
       </c>
       <c t="n" r="B13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C13">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c t="n" r="E13">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c s="1" t="n" r="A14">
-        <v>0.1143382949222053</v>
+        <v>0.06410720499822353</v>
       </c>
       <c t="n" r="B14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="D14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c s="1" t="n" r="A15">
-        <v>0.11635337949191546</v>
+        <v>0.08489057724821769</v>
       </c>
       <c t="n" r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="C15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="D15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E15">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c s="1" t="n" r="A16">
-        <v>0.11683845688364769</v>
+        <v>0.18184077197824708</v>
       </c>
       <c t="n" r="B16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="D16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E16">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c s="1" t="n" r="A17">
-        <v>0.12971370597969578</v>
+        <v>0.13022119317931488</v>
       </c>
       <c t="n" r="B17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="D17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c s="1" t="n" r="A18">
-        <v>0.13001694414860537</v>
+        <v>0.03457546063131148</v>
       </c>
       <c t="n" r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="C18">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c t="n" r="D18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="E18">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c s="1" t="n" r="A19">
-        <v>0.13022119317931488</v>
+        <v>0.0592547579755059</v>
       </c>
       <c t="n" r="B19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="D19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E19">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c s="1" t="n" r="A20">
-        <v>0.1477151116091055</v>
+        <v>0.060400417357177216</v>
       </c>
       <c t="n" r="B20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C20">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c t="n" r="D20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="E20">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c s="1" t="n" r="A21">
-        <v>0.14851510907452498</v>
+        <v>0.08597586519514165</v>
       </c>
       <c t="n" r="B21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c t="n" r="C21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="D21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E21">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c s="1" t="n" r="A22">
-        <v>0.14854446591931197</v>
+        <v>0.17908304986516244</v>
       </c>
       <c t="n" r="B22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C22">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c t="n" r="D22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E22">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c s="1" t="n" r="A23">
-        <v>0.14912278089866118</v>
+        <v>0.20966374631556323</v>
       </c>
       <c t="n" r="B23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C23">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="E23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c s="1" t="n" r="A24">
-        <v>0.16401741052103208</v>
+        <v>0.1477151116091055</v>
       </c>
       <c t="n" r="B24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="C24">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E24">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c s="1" t="n" r="A25">
-        <v>0.1659653838406194</v>
+        <v>0.19138675383684176</v>
       </c>
       <c t="n" r="B25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C25">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c t="n" r="E25">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c s="1" t="n" r="A26">
-        <v>0.1709028814756272</v>
+        <v>0.19121638516839604</v>
       </c>
       <c t="n" r="B26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="n" r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c s="1" t="n" r="A27">
-        <v>0.17908304986516244</v>
+        <v>0.19215024408228326</v>
       </c>
       <c t="n" r="B27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c t="n" r="C27">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c t="n" r="D27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E27">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c s="1" t="n" r="A28">
-        <v>0.18184077197824708</v>
+        <v>0.22143711641808975</v>
       </c>
       <c t="n" r="B28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C28">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c t="n" r="D28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E28">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c s="1" t="n" r="A29">
-        <v>0.19037965090090636</v>
+        <v>0.11683845688364769</v>
       </c>
       <c t="n" r="B29">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C29">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c t="n" r="D29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E29">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c s="1" t="n" r="A30">
-        <v>0.19121638516839604</v>
+        <v>0.2110846868384675</v>
       </c>
       <c t="n" r="B30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="C30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c t="n" r="D30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E30">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c s="1" t="n" r="A31">
-        <v>0.19138675383684176</v>
+        <v>0.23635579864455308</v>
       </c>
       <c t="n" r="B31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c t="n" r="C31">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c t="n" r="D31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E31">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c s="1" t="n" r="A32">
-        <v>0.19215024408228326</v>
+        <v>0.11635337949191546</v>
       </c>
       <c t="n" r="B32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C32">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c t="n" r="D32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="E32">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c s="1" t="n" r="A33">
-        <v>0.20966374631556323</v>
+        <v>0.050765735646263285</v>
       </c>
       <c t="n" r="B33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c t="n" r="C33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="D33">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E33">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c s="1" t="n" r="A34">
-        <v>0.2110846868384675</v>
+        <v>0.16401741052103208</v>
       </c>
       <c t="n" r="B34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C34">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c t="n" r="D34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c t="n" r="E34">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c s="1" t="n" r="A35">
-        <v>0.22143711641808975</v>
+        <v>0.1709028814756272</v>
       </c>
       <c t="n" r="B35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c t="n" r="C35">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E35">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c s="1" t="n" r="A36">
-        <v>0.23635579864455308</v>
+        <v>0.13001694414860537</v>
       </c>
       <c t="n" r="B36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c t="n" r="C36">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D36">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E36">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c s="1" t="n" r="A37">
-        <v>0.24919639115256959</v>
+        <v>0.14854446591931197</v>
       </c>
       <c t="n" r="B37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c t="n" r="C37">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c t="n" r="D37">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c t="n" r="E37">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>